<commit_message>
update of general development schedule
update of general development schedule 2025-06-01_0a0
</commit_message>
<xml_diff>
--- a/rocket build schedule 2025_0a0.xlsx
+++ b/rocket build schedule 2025_0a0.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xieyu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laptop0a1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16A4515-CD73-49C3-9851-EF6FA4E4689D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB59393-92FA-4FEF-93C7-3EF82989FCFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="32475" windowHeight="21210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="schedule and budget" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1249,7 +1249,7 @@
   <dimension ref="B2:NS222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="12.75"/>

</xml_diff>